<commit_message>
"working on 2001 - 2300
</commit_message>
<xml_diff>
--- a/payments.xlsx
+++ b/payments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Pay Tova</t>
   </si>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="H6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="I4" s="7">
         <f>SUM(I7:I16)</f>
-        <v>2240</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="5" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -681,7 +681,7 @@
         <v>1401</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" ref="H9:H16" si="2">G9+300-1</f>
+        <f t="shared" ref="H9:H15" si="2">G9+300-1</f>
         <v>1700</v>
       </c>
       <c r="I9" s="3">
@@ -903,7 +903,9 @@
         <f t="shared" si="2"/>
         <v>3500</v>
       </c>
-      <c r="I15" s="3"/>
+      <c r="I15" s="3">
+        <v>280</v>
+      </c>
       <c r="J15" s="9">
         <f t="shared" si="3"/>
         <v>2401</v>
@@ -912,6 +914,9 @@
         <f t="shared" si="4"/>
         <v>2700</v>
       </c>
+      <c r="L15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C16">
@@ -932,10 +937,13 @@
         <v>3501</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="2"/>
-        <v>3800</v>
-      </c>
-      <c r="I16" s="3"/>
+        <f>G16+390-1</f>
+        <v>3890</v>
+      </c>
+      <c r="I16" s="3">
+        <f>280*390/300</f>
+        <v>364</v>
+      </c>
       <c r="J16" s="9">
         <f t="shared" si="3"/>
         <v>2701</v>
@@ -944,8 +952,11 @@
         <f t="shared" si="4"/>
         <v>3000</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>2015</v>
       </c>
@@ -953,8 +964,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <f>SUM(I7:I16)</f>
+        <v>2884</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>2015</v>
       </c>
@@ -963,7 +978,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>2015</v>
       </c>
@@ -972,7 +987,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>2015</v>
       </c>
@@ -981,7 +996,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>2015</v>
       </c>
@@ -990,7 +1005,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>2015</v>
       </c>
@@ -999,7 +1014,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>2015</v>
       </c>
@@ -1008,7 +1023,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>2015</v>
       </c>
@@ -1017,7 +1032,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>2015</v>
       </c>
@@ -1026,7 +1041,7 @@
       </c>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>2015</v>
       </c>
@@ -1035,7 +1050,7 @@
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>2015</v>
       </c>
@@ -1044,7 +1059,7 @@
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>2015</v>
       </c>
@@ -1053,7 +1068,7 @@
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>2015</v>
       </c>
@@ -1062,7 +1077,7 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>2015</v>
       </c>

</xml_diff>